<commit_message>
firebase fileuploading and other features implemented
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New File</t>
   </si>
 </sst>
 </file>
@@ -183,11 +186,11 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" t="s" s="0">
-        <v>8</v>
+      <c r="A1" s="0">
+        <v>10.26</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -197,12 +200,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>19</v>
-      </c>
+      <c r="A2" s="0">
+        <v>20.12</v>
+      </c>
+      <c r="B2" s="0"/>
       <c r="C2" t="s">
         <v>12</v>
       </c>
@@ -211,12 +212,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
+      <c r="A3" s="0">
+        <v>30.01</v>
+      </c>
+      <c r="B3" s="0"/>
       <c r="C3" t="s">
         <v>14</v>
       </c>
@@ -225,12 +224,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
+      <c r="A4">
+        <v>40.29</v>
+      </c>
+      <c r="B4"/>
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -239,12 +236,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5">
+        <v>50.18</v>
+      </c>
+      <c r="B5"/>
       <c r="C5" t="s">
         <v>18</v>
       </c>

</xml_diff>